<commit_message>
Añadidas mas fechas de entrega y presentación
</commit_message>
<xml_diff>
--- a/PropuestaProyecto/cronograma.xlsx
+++ b/PropuestaProyecto/cronograma.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>N.º</t>
   </si>
@@ -40,12 +40,6 @@
     <t>Presupuesto</t>
   </si>
   <si>
-    <t>BD</t>
-  </si>
-  <si>
-    <t>Casos de uso</t>
-  </si>
-  <si>
     <t>Objeto de la propuesta</t>
   </si>
   <si>
@@ -60,12 +54,36 @@
   <si>
     <t>Documentación</t>
   </si>
+  <si>
+    <t>BD (implementacion)</t>
+  </si>
+  <si>
+    <t>BD (diseño)</t>
+  </si>
+  <si>
+    <t>Propuesta de proyecto</t>
+  </si>
+  <si>
+    <t>Segunda iteración</t>
+  </si>
+  <si>
+    <t>Presentación comercial del proyecto</t>
+  </si>
+  <si>
+    <t>Presentación técnica del proyecto</t>
+  </si>
+  <si>
+    <t>Entrega del proyecto</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -88,8 +106,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,6 +191,36 @@
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.499984740745262"/>
         <bgColor indexed="26"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -344,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -385,9 +440,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -411,6 +463,25 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,7 +842,7 @@
   <dimension ref="A1:IV34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+      <selection activeCell="DA24" sqref="DA24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -784,173 +855,173 @@
   <sheetData>
     <row r="1" spans="1:256" ht="9.9499999999999993" customHeight="1"/>
     <row r="2" spans="1:256" s="1" customFormat="1" ht="17.850000000000001" customHeight="1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="20"/>
-      <c r="AD2" s="20"/>
-      <c r="AE2" s="20"/>
-      <c r="AF2" s="20" t="s">
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="41"/>
+      <c r="V2" s="41"/>
+      <c r="W2" s="41"/>
+      <c r="X2" s="41"/>
+      <c r="Y2" s="41"/>
+      <c r="Z2" s="41"/>
+      <c r="AA2" s="41"/>
+      <c r="AB2" s="41"/>
+      <c r="AC2" s="41"/>
+      <c r="AD2" s="41"/>
+      <c r="AE2" s="41"/>
+      <c r="AF2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="20"/>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="20"/>
-      <c r="AL2" s="20"/>
-      <c r="AM2" s="20"/>
-      <c r="AN2" s="20"/>
-      <c r="AO2" s="20"/>
-      <c r="AP2" s="20"/>
-      <c r="AQ2" s="20"/>
-      <c r="AR2" s="20"/>
-      <c r="AS2" s="20"/>
-      <c r="AT2" s="20"/>
-      <c r="AU2" s="20"/>
-      <c r="AV2" s="20"/>
-      <c r="AW2" s="20"/>
-      <c r="AX2" s="20"/>
-      <c r="AY2" s="20"/>
-      <c r="AZ2" s="20"/>
-      <c r="BA2" s="20"/>
-      <c r="BB2" s="20"/>
-      <c r="BC2" s="20"/>
-      <c r="BD2" s="20"/>
-      <c r="BE2" s="20"/>
-      <c r="BF2" s="20"/>
-      <c r="BG2" s="20"/>
-      <c r="BH2" s="20"/>
-      <c r="BI2" s="20"/>
-      <c r="BJ2" s="20"/>
-      <c r="BK2" s="20" t="s">
+      <c r="AG2" s="41"/>
+      <c r="AH2" s="41"/>
+      <c r="AI2" s="41"/>
+      <c r="AJ2" s="41"/>
+      <c r="AK2" s="41"/>
+      <c r="AL2" s="41"/>
+      <c r="AM2" s="41"/>
+      <c r="AN2" s="41"/>
+      <c r="AO2" s="41"/>
+      <c r="AP2" s="41"/>
+      <c r="AQ2" s="41"/>
+      <c r="AR2" s="41"/>
+      <c r="AS2" s="41"/>
+      <c r="AT2" s="41"/>
+      <c r="AU2" s="41"/>
+      <c r="AV2" s="41"/>
+      <c r="AW2" s="41"/>
+      <c r="AX2" s="41"/>
+      <c r="AY2" s="41"/>
+      <c r="AZ2" s="41"/>
+      <c r="BA2" s="41"/>
+      <c r="BB2" s="41"/>
+      <c r="BC2" s="41"/>
+      <c r="BD2" s="41"/>
+      <c r="BE2" s="41"/>
+      <c r="BF2" s="41"/>
+      <c r="BG2" s="41"/>
+      <c r="BH2" s="41"/>
+      <c r="BI2" s="41"/>
+      <c r="BJ2" s="41"/>
+      <c r="BK2" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="BL2" s="20"/>
-      <c r="BM2" s="20"/>
-      <c r="BN2" s="20"/>
-      <c r="BO2" s="20"/>
-      <c r="BP2" s="20"/>
-      <c r="BQ2" s="20"/>
-      <c r="BR2" s="20"/>
-      <c r="BS2" s="20"/>
-      <c r="BT2" s="20"/>
-      <c r="BU2" s="20"/>
-      <c r="BV2" s="20"/>
-      <c r="BW2" s="20"/>
-      <c r="BX2" s="20"/>
-      <c r="BY2" s="20"/>
-      <c r="BZ2" s="20"/>
-      <c r="CA2" s="20"/>
-      <c r="CB2" s="20"/>
-      <c r="CC2" s="20"/>
-      <c r="CD2" s="20"/>
-      <c r="CE2" s="20"/>
-      <c r="CF2" s="20"/>
-      <c r="CG2" s="20"/>
-      <c r="CH2" s="20"/>
-      <c r="CI2" s="20"/>
-      <c r="CJ2" s="20"/>
-      <c r="CK2" s="20"/>
-      <c r="CL2" s="20"/>
-      <c r="CM2" s="20"/>
-      <c r="CN2" s="20"/>
-      <c r="CO2" s="20" t="s">
+      <c r="BL2" s="41"/>
+      <c r="BM2" s="41"/>
+      <c r="BN2" s="41"/>
+      <c r="BO2" s="41"/>
+      <c r="BP2" s="41"/>
+      <c r="BQ2" s="41"/>
+      <c r="BR2" s="41"/>
+      <c r="BS2" s="41"/>
+      <c r="BT2" s="41"/>
+      <c r="BU2" s="41"/>
+      <c r="BV2" s="41"/>
+      <c r="BW2" s="41"/>
+      <c r="BX2" s="41"/>
+      <c r="BY2" s="41"/>
+      <c r="BZ2" s="41"/>
+      <c r="CA2" s="41"/>
+      <c r="CB2" s="41"/>
+      <c r="CC2" s="41"/>
+      <c r="CD2" s="41"/>
+      <c r="CE2" s="41"/>
+      <c r="CF2" s="41"/>
+      <c r="CG2" s="41"/>
+      <c r="CH2" s="41"/>
+      <c r="CI2" s="41"/>
+      <c r="CJ2" s="41"/>
+      <c r="CK2" s="41"/>
+      <c r="CL2" s="41"/>
+      <c r="CM2" s="41"/>
+      <c r="CN2" s="41"/>
+      <c r="CO2" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="CP2" s="20"/>
-      <c r="CQ2" s="20"/>
-      <c r="CR2" s="20"/>
-      <c r="CS2" s="20"/>
-      <c r="CT2" s="20"/>
-      <c r="CU2" s="20"/>
-      <c r="CV2" s="20"/>
-      <c r="CW2" s="20"/>
-      <c r="CX2" s="20"/>
-      <c r="CY2" s="20"/>
-      <c r="CZ2" s="20"/>
-      <c r="DA2" s="20"/>
-      <c r="DB2" s="20"/>
-      <c r="DC2" s="20"/>
-      <c r="DD2" s="20"/>
-      <c r="DE2" s="20"/>
-      <c r="DF2" s="20"/>
-      <c r="DG2" s="20"/>
-      <c r="DH2" s="20"/>
-      <c r="DI2" s="20"/>
-      <c r="DJ2" s="20"/>
-      <c r="DK2" s="20"/>
-      <c r="DL2" s="20"/>
-      <c r="DM2" s="20"/>
-      <c r="DN2" s="20"/>
-      <c r="DO2" s="20"/>
-      <c r="DP2" s="20"/>
-      <c r="DQ2" s="20"/>
-      <c r="DR2" s="20"/>
-      <c r="DS2" s="20"/>
-      <c r="DT2" s="20" t="s">
+      <c r="CP2" s="41"/>
+      <c r="CQ2" s="41"/>
+      <c r="CR2" s="41"/>
+      <c r="CS2" s="41"/>
+      <c r="CT2" s="41"/>
+      <c r="CU2" s="41"/>
+      <c r="CV2" s="41"/>
+      <c r="CW2" s="41"/>
+      <c r="CX2" s="41"/>
+      <c r="CY2" s="41"/>
+      <c r="CZ2" s="41"/>
+      <c r="DA2" s="41"/>
+      <c r="DB2" s="41"/>
+      <c r="DC2" s="41"/>
+      <c r="DD2" s="41"/>
+      <c r="DE2" s="41"/>
+      <c r="DF2" s="41"/>
+      <c r="DG2" s="41"/>
+      <c r="DH2" s="41"/>
+      <c r="DI2" s="41"/>
+      <c r="DJ2" s="41"/>
+      <c r="DK2" s="41"/>
+      <c r="DL2" s="41"/>
+      <c r="DM2" s="41"/>
+      <c r="DN2" s="41"/>
+      <c r="DO2" s="41"/>
+      <c r="DP2" s="41"/>
+      <c r="DQ2" s="41"/>
+      <c r="DR2" s="41"/>
+      <c r="DS2" s="41"/>
+      <c r="DT2" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="DU2" s="20"/>
-      <c r="DV2" s="20"/>
-      <c r="DW2" s="20"/>
-      <c r="DX2" s="20"/>
-      <c r="DY2" s="20"/>
-      <c r="DZ2" s="20"/>
-      <c r="EA2" s="20"/>
-      <c r="EB2" s="20"/>
-      <c r="EC2" s="20"/>
-      <c r="ED2" s="20"/>
-      <c r="EE2" s="20"/>
-      <c r="EF2" s="20"/>
-      <c r="EG2" s="20"/>
-      <c r="EH2" s="20"/>
-      <c r="EI2" s="20"/>
-      <c r="EJ2" s="20"/>
-      <c r="EK2" s="20"/>
-      <c r="EL2" s="20"/>
-      <c r="EM2" s="20"/>
-      <c r="EN2" s="20"/>
-      <c r="EO2" s="20"/>
-      <c r="EP2" s="20"/>
-      <c r="EQ2" s="20"/>
-      <c r="ER2" s="20"/>
-      <c r="ES2" s="20"/>
-      <c r="ET2" s="20"/>
-      <c r="EU2" s="20"/>
-      <c r="EV2" s="20"/>
-      <c r="EW2" s="20"/>
+      <c r="DU2" s="41"/>
+      <c r="DV2" s="41"/>
+      <c r="DW2" s="41"/>
+      <c r="DX2" s="41"/>
+      <c r="DY2" s="41"/>
+      <c r="DZ2" s="41"/>
+      <c r="EA2" s="41"/>
+      <c r="EB2" s="41"/>
+      <c r="EC2" s="41"/>
+      <c r="ED2" s="41"/>
+      <c r="EE2" s="41"/>
+      <c r="EF2" s="41"/>
+      <c r="EG2" s="41"/>
+      <c r="EH2" s="41"/>
+      <c r="EI2" s="41"/>
+      <c r="EJ2" s="41"/>
+      <c r="EK2" s="41"/>
+      <c r="EL2" s="41"/>
+      <c r="EM2" s="41"/>
+      <c r="EN2" s="41"/>
+      <c r="EO2" s="41"/>
+      <c r="EP2" s="41"/>
+      <c r="EQ2" s="41"/>
+      <c r="ER2" s="41"/>
+      <c r="ES2" s="41"/>
+      <c r="ET2" s="41"/>
+      <c r="EU2" s="41"/>
+      <c r="EV2" s="41"/>
+      <c r="EW2" s="41"/>
       <c r="EX2"/>
       <c r="EY2"/>
       <c r="EZ2"/>
@@ -1056,8 +1127,8 @@
       <c r="IV2"/>
     </row>
     <row r="3" spans="1:256">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
       <c r="C3" s="2">
         <v>1</v>
       </c>
@@ -1517,44 +1588,44 @@
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="10"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="22"/>
-      <c r="V4" s="22"/>
-      <c r="W4" s="22"/>
-      <c r="X4" s="22"/>
-      <c r="Y4" s="22"/>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="22"/>
-      <c r="AB4" s="34"/>
-      <c r="AC4" s="22"/>
-      <c r="AD4" s="22"/>
-      <c r="AE4" s="35"/>
-      <c r="AF4" s="36"/>
-      <c r="AG4" s="22"/>
-      <c r="AH4" s="22"/>
-      <c r="AI4" s="22"/>
-      <c r="AJ4" s="22"/>
-      <c r="AK4" s="22"/>
-      <c r="AL4" s="22"/>
-      <c r="AM4" s="22"/>
-      <c r="AN4" s="22"/>
-      <c r="AO4" s="22"/>
-      <c r="AP4" s="22"/>
-      <c r="AQ4" s="22"/>
-      <c r="AR4" s="22"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="21"/>
+      <c r="W4" s="21"/>
+      <c r="X4" s="21"/>
+      <c r="Y4" s="21"/>
+      <c r="Z4" s="21"/>
+      <c r="AA4" s="21"/>
+      <c r="AB4" s="33"/>
+      <c r="AC4" s="21"/>
+      <c r="AD4" s="21"/>
+      <c r="AE4" s="34"/>
+      <c r="AF4" s="35"/>
+      <c r="AG4" s="21"/>
+      <c r="AH4" s="21"/>
+      <c r="AI4" s="36"/>
+      <c r="AJ4" s="36"/>
+      <c r="AK4" s="36"/>
+      <c r="AL4" s="36"/>
+      <c r="AM4" s="36"/>
+      <c r="AN4" s="36"/>
+      <c r="AO4" s="36"/>
+      <c r="AP4" s="36"/>
+      <c r="AQ4" s="36"/>
+      <c r="AR4" s="36"/>
       <c r="BJ4" s="12"/>
       <c r="BK4" s="10"/>
       <c r="CO4" s="10"/>
@@ -1670,17 +1741,17 @@
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="10"/>
-      <c r="Q5" s="39"/>
-      <c r="R5" s="39"/>
-      <c r="S5" s="39"/>
-      <c r="T5" s="39"/>
-      <c r="U5" s="39"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="38"/>
       <c r="AE5" s="12"/>
       <c r="AF5" s="10"/>
-      <c r="AO5" s="37"/>
+      <c r="AO5" s="36"/>
       <c r="BJ5" s="12"/>
       <c r="BK5" s="10"/>
       <c r="CO5" s="10"/>
@@ -1796,28 +1867,28 @@
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="10"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="23"/>
-      <c r="X6" s="23"/>
-      <c r="Y6" s="23"/>
-      <c r="Z6" s="23"/>
-      <c r="AA6" s="23"/>
-      <c r="AB6" s="23"/>
-      <c r="AC6" s="23"/>
-      <c r="AD6" s="23"/>
-      <c r="AE6" s="24"/>
-      <c r="AF6" s="25"/>
-      <c r="AG6" s="23"/>
-      <c r="AH6" s="23"/>
-      <c r="AI6" s="23"/>
-      <c r="AJ6" s="23"/>
-      <c r="AK6" s="23"/>
-      <c r="AL6" s="23"/>
+      <c r="T6" s="22"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="22"/>
+      <c r="Y6" s="22"/>
+      <c r="Z6" s="22"/>
+      <c r="AA6" s="22"/>
+      <c r="AB6" s="22"/>
+      <c r="AC6" s="22"/>
+      <c r="AD6" s="22"/>
+      <c r="AE6" s="23"/>
+      <c r="AF6" s="24"/>
+      <c r="AG6" s="22"/>
+      <c r="AH6" s="22"/>
+      <c r="AI6" s="22"/>
+      <c r="AJ6" s="22"/>
+      <c r="AK6" s="22"/>
+      <c r="AL6" s="22"/>
       <c r="BJ6" s="12"/>
       <c r="BK6" s="10"/>
       <c r="CO6" s="10"/>
@@ -1933,13 +2004,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" s="10"/>
       <c r="AE7" s="12"/>
       <c r="AF7" s="10"/>
-      <c r="AN7" s="26"/>
-      <c r="AO7" s="26"/>
+      <c r="AN7" s="25"/>
+      <c r="AO7" s="25"/>
       <c r="BJ7" s="12"/>
       <c r="BK7" s="10"/>
       <c r="CO7" s="10"/>
@@ -2055,22 +2126,22 @@
         <v>5</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C8" s="10"/>
       <c r="AE8" s="12"/>
       <c r="AF8" s="10"/>
-      <c r="AH8" s="28"/>
-      <c r="AI8" s="28"/>
-      <c r="AJ8" s="28"/>
-      <c r="AK8" s="28"/>
-      <c r="AL8" s="28"/>
-      <c r="AM8" s="28"/>
-      <c r="AN8" s="28"/>
-      <c r="AO8" s="28"/>
-      <c r="AP8" s="28"/>
-      <c r="AQ8" s="28"/>
-      <c r="AR8" s="28"/>
+      <c r="AH8" s="27"/>
+      <c r="AI8" s="27"/>
+      <c r="AJ8" s="27"/>
+      <c r="AK8" s="27"/>
+      <c r="AL8" s="27"/>
+      <c r="AM8" s="27"/>
+      <c r="AN8" s="27"/>
+      <c r="AO8" s="27"/>
+      <c r="AP8" s="36"/>
+      <c r="AQ8" s="36"/>
+      <c r="AR8" s="36"/>
       <c r="BJ8" s="12"/>
       <c r="BK8" s="10"/>
       <c r="CO8" s="10"/>
@@ -2186,15 +2257,29 @@
         <v>6</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C9" s="10"/>
       <c r="AE9" s="12"/>
       <c r="AF9" s="10"/>
-      <c r="AO9" s="31"/>
-      <c r="AP9" s="31"/>
-      <c r="AQ9" s="31"/>
-      <c r="AR9" s="31"/>
+      <c r="AH9" s="30"/>
+      <c r="AI9" s="30"/>
+      <c r="AJ9" s="30"/>
+      <c r="AK9" s="30"/>
+      <c r="AL9" s="30"/>
+      <c r="AM9" s="30"/>
+      <c r="AN9" s="30"/>
+      <c r="AO9" s="30"/>
+      <c r="AP9" s="30"/>
+      <c r="AQ9" s="30"/>
+      <c r="AR9" s="30"/>
+      <c r="AS9" s="30"/>
+      <c r="AT9" s="30"/>
+      <c r="AU9" s="30"/>
+      <c r="AV9" s="30"/>
+      <c r="AW9" s="30"/>
+      <c r="AX9" s="30"/>
+      <c r="AY9" s="30"/>
       <c r="BJ9" s="12"/>
       <c r="BK9" s="10"/>
       <c r="CO9" s="10"/>
@@ -2313,19 +2398,19 @@
         <v>7</v>
       </c>
       <c r="C10" s="10"/>
-      <c r="AE10" s="32"/>
-      <c r="AF10" s="33"/>
-      <c r="AG10" s="27"/>
-      <c r="AH10" s="27"/>
-      <c r="AI10" s="27"/>
-      <c r="AJ10" s="27"/>
-      <c r="AK10" s="27"/>
-      <c r="AL10" s="27"/>
-      <c r="AM10" s="27"/>
-      <c r="AN10" s="27"/>
-      <c r="AO10" s="27"/>
-      <c r="AP10" s="27"/>
-      <c r="AQ10" s="27"/>
+      <c r="AE10" s="31"/>
+      <c r="AF10" s="32"/>
+      <c r="AG10" s="26"/>
+      <c r="AH10" s="26"/>
+      <c r="AI10" s="26"/>
+      <c r="AJ10" s="26"/>
+      <c r="AK10" s="26"/>
+      <c r="AL10" s="26"/>
+      <c r="AM10" s="26"/>
+      <c r="AN10" s="26"/>
+      <c r="AO10" s="26"/>
+      <c r="AP10" s="26"/>
+      <c r="AQ10" s="26"/>
       <c r="BJ10" s="12"/>
       <c r="BK10" s="10"/>
       <c r="CO10" s="10"/>
@@ -2441,47 +2526,121 @@
         <v>8</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11" s="10"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="38"/>
-      <c r="S11" s="38"/>
-      <c r="T11" s="38"/>
-      <c r="U11" s="38"/>
-      <c r="V11" s="38"/>
-      <c r="W11" s="38"/>
-      <c r="X11" s="38"/>
-      <c r="Y11" s="38"/>
-      <c r="Z11" s="38"/>
-      <c r="AA11" s="38"/>
-      <c r="AB11" s="38"/>
-      <c r="AC11" s="38"/>
-      <c r="AD11" s="38"/>
-      <c r="AE11" s="40"/>
-      <c r="AF11" s="41"/>
-      <c r="AG11" s="38"/>
-      <c r="AH11" s="38"/>
-      <c r="AI11" s="38"/>
-      <c r="AJ11" s="38"/>
-      <c r="AK11" s="38"/>
-      <c r="AL11" s="38"/>
-      <c r="AM11" s="38"/>
-      <c r="AN11" s="38"/>
-      <c r="AO11" s="38"/>
-      <c r="AP11" s="38"/>
-      <c r="AQ11" s="38"/>
-      <c r="AR11" s="38"/>
-      <c r="BJ11" s="12"/>
-      <c r="BK11" s="10"/>
-      <c r="CO11" s="10"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="37"/>
+      <c r="R11" s="37"/>
+      <c r="S11" s="37"/>
+      <c r="T11" s="37"/>
+      <c r="U11" s="37"/>
+      <c r="V11" s="37"/>
+      <c r="W11" s="37"/>
+      <c r="X11" s="37"/>
+      <c r="Y11" s="37"/>
+      <c r="Z11" s="37"/>
+      <c r="AA11" s="37"/>
+      <c r="AB11" s="37"/>
+      <c r="AC11" s="37"/>
+      <c r="AD11" s="37"/>
+      <c r="AE11" s="39"/>
+      <c r="AF11" s="40"/>
+      <c r="AG11" s="37"/>
+      <c r="AH11" s="37"/>
+      <c r="AI11" s="37"/>
+      <c r="AJ11" s="37"/>
+      <c r="AK11" s="37"/>
+      <c r="AL11" s="37"/>
+      <c r="AM11" s="37"/>
+      <c r="AN11" s="37"/>
+      <c r="AO11" s="37"/>
+      <c r="AP11" s="37"/>
+      <c r="AQ11" s="37"/>
+      <c r="AR11" s="37"/>
+      <c r="AS11" s="37"/>
+      <c r="AT11" s="37"/>
+      <c r="AU11" s="37"/>
+      <c r="AV11" s="37"/>
+      <c r="AW11" s="37"/>
+      <c r="AX11" s="37"/>
+      <c r="AY11" s="37"/>
+      <c r="AZ11" s="37"/>
+      <c r="BA11" s="37"/>
+      <c r="BB11" s="37"/>
+      <c r="BC11" s="37"/>
+      <c r="BD11" s="37"/>
+      <c r="BE11" s="37"/>
+      <c r="BF11" s="37"/>
+      <c r="BG11" s="37"/>
+      <c r="BH11" s="37"/>
+      <c r="BI11" s="37"/>
+      <c r="BJ11" s="39"/>
+      <c r="BK11" s="40"/>
+      <c r="BL11" s="37"/>
+      <c r="BM11" s="37"/>
+      <c r="BN11" s="37"/>
+      <c r="BO11" s="37"/>
+      <c r="BP11" s="37"/>
+      <c r="BQ11" s="37"/>
+      <c r="BR11" s="37"/>
+      <c r="BS11" s="37"/>
+      <c r="BT11" s="37"/>
+      <c r="BU11" s="37"/>
+      <c r="BV11" s="37"/>
+      <c r="BW11" s="37"/>
+      <c r="BX11" s="37"/>
+      <c r="BY11" s="37"/>
+      <c r="BZ11" s="37"/>
+      <c r="CA11" s="37"/>
+      <c r="CB11" s="37"/>
+      <c r="CC11" s="37"/>
+      <c r="CD11" s="37"/>
+      <c r="CE11" s="37"/>
+      <c r="CF11" s="37"/>
+      <c r="CG11" s="37"/>
+      <c r="CH11" s="37"/>
+      <c r="CI11" s="37"/>
+      <c r="CJ11" s="37"/>
+      <c r="CK11" s="37"/>
+      <c r="CL11" s="37"/>
+      <c r="CM11" s="37"/>
+      <c r="CN11" s="37"/>
+      <c r="CO11" s="40"/>
+      <c r="CP11" s="37"/>
+      <c r="CQ11" s="37"/>
+      <c r="CR11" s="37"/>
+      <c r="CS11" s="37"/>
+      <c r="CT11" s="37"/>
+      <c r="CU11" s="37"/>
+      <c r="CV11" s="37"/>
+      <c r="CW11" s="37"/>
+      <c r="CX11" s="37"/>
+      <c r="CY11" s="37"/>
+      <c r="CZ11" s="37"/>
+      <c r="DA11" s="37"/>
+      <c r="DB11" s="37"/>
+      <c r="DC11" s="37"/>
+      <c r="DD11" s="37"/>
+      <c r="DE11" s="37"/>
+      <c r="DF11" s="37"/>
+      <c r="DG11" s="37"/>
+      <c r="DH11" s="37"/>
+      <c r="DI11" s="37"/>
+      <c r="DJ11" s="37"/>
+      <c r="DK11" s="37"/>
+      <c r="DL11" s="37"/>
+      <c r="DM11" s="37"/>
+      <c r="DN11" s="37"/>
+      <c r="DO11" s="37"/>
+      <c r="DP11" s="36"/>
+      <c r="DQ11" s="36"/>
       <c r="DS11" s="12"/>
       <c r="DT11" s="10"/>
       <c r="EW11" s="12"/>
@@ -2593,10 +2752,45 @@
       <c r="A12" s="9">
         <v>9</v>
       </c>
+      <c r="B12" s="42" t="s">
+        <v>15</v>
+      </c>
       <c r="C12" s="13"/>
-      <c r="AE12" s="15"/>
-      <c r="AF12" s="13"/>
-      <c r="AQ12" s="21"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="43"/>
+      <c r="T12" s="43"/>
+      <c r="U12" s="43"/>
+      <c r="V12" s="43"/>
+      <c r="W12" s="43"/>
+      <c r="X12" s="43"/>
+      <c r="Y12" s="43"/>
+      <c r="Z12" s="43"/>
+      <c r="AA12" s="43"/>
+      <c r="AB12" s="43"/>
+      <c r="AC12" s="43"/>
+      <c r="AD12" s="43"/>
+      <c r="AE12" s="44"/>
+      <c r="AF12" s="45"/>
+      <c r="AG12" s="43"/>
+      <c r="AH12" s="43"/>
+      <c r="AI12" s="43"/>
+      <c r="AJ12" s="43"/>
+      <c r="AK12" s="43"/>
+      <c r="AL12" s="43"/>
+      <c r="AM12" s="43"/>
+      <c r="AN12" s="43"/>
+      <c r="AO12" s="43"/>
+      <c r="AP12" s="43"/>
+      <c r="AQ12" s="46"/>
+      <c r="AR12" s="43"/>
       <c r="BJ12" s="15"/>
       <c r="BK12" s="13"/>
       <c r="CO12" s="13"/>
@@ -2711,13 +2905,54 @@
       <c r="A13" s="9">
         <v>10</v>
       </c>
+      <c r="B13" s="42" t="s">
+        <v>16</v>
+      </c>
       <c r="C13" s="13"/>
       <c r="AE13" s="15"/>
       <c r="AF13" s="13"/>
-      <c r="AQ13" s="21"/>
-      <c r="BJ13" s="15"/>
-      <c r="BK13" s="13"/>
-      <c r="CO13" s="13"/>
+      <c r="AQ13" s="20"/>
+      <c r="BC13" s="28"/>
+      <c r="BD13" s="28"/>
+      <c r="BE13" s="28"/>
+      <c r="BF13" s="28"/>
+      <c r="BG13" s="28"/>
+      <c r="BH13" s="28"/>
+      <c r="BI13" s="28"/>
+      <c r="BJ13" s="49"/>
+      <c r="BK13" s="50"/>
+      <c r="BL13" s="28"/>
+      <c r="BM13" s="28"/>
+      <c r="BN13" s="28"/>
+      <c r="BO13" s="28"/>
+      <c r="BP13" s="28"/>
+      <c r="BQ13" s="28"/>
+      <c r="BR13" s="28"/>
+      <c r="BS13" s="28"/>
+      <c r="BT13" s="28"/>
+      <c r="BU13" s="28"/>
+      <c r="BV13" s="28"/>
+      <c r="BW13" s="28"/>
+      <c r="BX13" s="28"/>
+      <c r="BY13" s="28"/>
+      <c r="BZ13" s="28"/>
+      <c r="CA13" s="28"/>
+      <c r="CB13" s="47"/>
+      <c r="CC13" s="47"/>
+      <c r="CD13" s="47"/>
+      <c r="CE13" s="47"/>
+      <c r="CF13" s="47"/>
+      <c r="CG13" s="47"/>
+      <c r="CH13" s="47"/>
+      <c r="CI13" s="47"/>
+      <c r="CJ13" s="47"/>
+      <c r="CK13" s="47"/>
+      <c r="CL13" s="47"/>
+      <c r="CM13" s="47"/>
+      <c r="CN13" s="47"/>
+      <c r="CO13" s="48"/>
+      <c r="CP13" s="47"/>
+      <c r="CQ13" s="47"/>
       <c r="DS13" s="15"/>
       <c r="DT13" s="13"/>
       <c r="EW13" s="15"/>
@@ -2829,13 +3064,21 @@
       <c r="A14" s="9">
         <v>11</v>
       </c>
+      <c r="B14" s="42" t="s">
+        <v>17</v>
+      </c>
       <c r="C14" s="13"/>
       <c r="AE14" s="15"/>
       <c r="AF14" s="13"/>
-      <c r="AQ14" s="21"/>
+      <c r="AQ14" s="20"/>
       <c r="BJ14" s="15"/>
       <c r="BK14" s="13"/>
       <c r="CO14" s="13"/>
+      <c r="CW14" s="51"/>
+      <c r="CX14" s="51"/>
+      <c r="CY14" s="51"/>
+      <c r="CZ14" s="51"/>
+      <c r="DA14" s="51"/>
       <c r="DS14" s="15"/>
       <c r="DT14" s="13"/>
       <c r="EW14" s="15"/>
@@ -2947,23 +3190,30 @@
       <c r="A15" s="9">
         <v>12</v>
       </c>
-      <c r="B15" s="9"/>
+      <c r="B15" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="C15" s="13"/>
       <c r="AE15" s="15"/>
       <c r="AF15" s="13"/>
-      <c r="AH15" s="29"/>
-      <c r="AI15" s="29"/>
-      <c r="AJ15" s="29"/>
-      <c r="AK15" s="29"/>
-      <c r="AL15" s="29"/>
-      <c r="AM15" s="29"/>
-      <c r="AN15" s="29"/>
-      <c r="AO15" s="29"/>
-      <c r="AP15" s="29"/>
-      <c r="AQ15" s="30"/>
+      <c r="AH15" s="28"/>
+      <c r="AI15" s="28"/>
+      <c r="AJ15" s="28"/>
+      <c r="AK15" s="28"/>
+      <c r="AL15" s="28"/>
+      <c r="AM15" s="28"/>
+      <c r="AN15" s="28"/>
+      <c r="AO15" s="28"/>
+      <c r="AP15" s="28"/>
+      <c r="AQ15" s="29"/>
       <c r="BJ15" s="15"/>
       <c r="BK15" s="13"/>
       <c r="CO15" s="13"/>
+      <c r="DK15" s="52"/>
+      <c r="DL15" s="52"/>
+      <c r="DM15" s="52"/>
+      <c r="DN15" s="52"/>
+      <c r="DO15" s="52"/>
       <c r="DS15" s="15"/>
       <c r="DT15" s="13"/>
       <c r="EW15" s="15"/>
@@ -3075,13 +3325,18 @@
       <c r="A16" s="9">
         <v>13</v>
       </c>
-      <c r="B16" s="9"/>
+      <c r="B16" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="C16" s="13"/>
       <c r="AE16" s="15"/>
       <c r="AF16" s="13"/>
       <c r="BJ16" s="15"/>
       <c r="BK16" s="13"/>
       <c r="CO16" s="13"/>
+      <c r="DO16" s="53" t="s">
+        <v>20</v>
+      </c>
       <c r="DS16" s="15"/>
       <c r="DT16" s="13"/>
       <c r="EW16" s="15"/>

</xml_diff>